<commit_message>
docs: update demo content
</commit_message>
<xml_diff>
--- a/excel-fixtures/Journyx_report_20190812.xlsx
+++ b/excel-fixtures/Journyx_report_20190812.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22005"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22010"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/peterbiermann/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="107" documentId="8_{892D9832-0701-4149-AEF8-7C7282F96FA5}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{C7A56AB2-5719-44AC-8FAA-FC31ECF410D9}"/>
+  <xr:revisionPtr revIDLastSave="275" documentId="8_{892D9832-0701-4149-AEF8-7C7282F96FA5}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{B5F908CB-0733-49D6-8824-56F7465718C4}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="40960" windowHeight="23040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
   <si>
     <t>Pay Roll Report</t>
   </si>
@@ -57,26 +57,17 @@
     <t>Pay Type</t>
   </si>
   <si>
-    <t>D.5 - Half-day holiday</t>
-  </si>
-  <si>
-    <t>NNAD - Unpaid overtime</t>
-  </si>
-  <si>
-    <t>NV - Compensatory leave</t>
-  </si>
-  <si>
-    <t>PUBLIC HOLIDAY</t>
-  </si>
-  <si>
-    <t>T: - Time in work</t>
+    <t>Total Expected</t>
+  </si>
+  <si>
+    <t>Result</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -87,6 +78,13 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -112,12 +110,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -484,7 +483,7 @@
   <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13:H19"/>
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -534,8 +533,8 @@
       </c>
     </row>
     <row r="7" spans="1:7">
-      <c r="A7" t="s">
-        <v>9</v>
+      <c r="A7">
+        <v>1</v>
       </c>
       <c r="C7" s="1">
         <v>0</v>
@@ -554,8 +553,8 @@
       </c>
     </row>
     <row r="8" spans="1:7">
-      <c r="A8" t="s">
-        <v>10</v>
+      <c r="A8">
+        <v>2</v>
       </c>
       <c r="C8" s="1">
         <v>1</v>
@@ -574,8 +573,8 @@
       </c>
     </row>
     <row r="9" spans="1:7">
-      <c r="A9" t="s">
-        <v>11</v>
+      <c r="A9">
+        <v>3</v>
       </c>
       <c r="C9" s="1">
         <v>0</v>
@@ -594,8 +593,8 @@
       </c>
     </row>
     <row r="10" spans="1:7">
-      <c r="A10" t="s">
-        <v>12</v>
+      <c r="A10">
+        <v>4</v>
       </c>
       <c r="C10" s="1">
         <v>16</v>
@@ -614,8 +613,8 @@
       </c>
     </row>
     <row r="11" spans="1:7">
-      <c r="A11" t="s">
-        <v>13</v>
+      <c r="A11">
+        <v>5</v>
       </c>
       <c r="C11" s="1">
         <v>8</v>
@@ -654,14 +653,38 @@
       </c>
     </row>
     <row r="14" spans="1:7">
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
-      <c r="F14" s="2"/>
+      <c r="A14" t="s">
+        <v>9</v>
+      </c>
+      <c r="C14" s="3">
+        <v>168</v>
+      </c>
+      <c r="D14" s="3">
+        <v>168</v>
+      </c>
+      <c r="E14" s="3">
+        <v>168</v>
+      </c>
+      <c r="F14" s="3">
+        <v>168</v>
+      </c>
     </row>
     <row r="15" spans="1:7">
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
-      <c r="F15" s="2"/>
+      <c r="A15" t="s">
+        <v>10</v>
+      </c>
+      <c r="C15" s="2">
+        <v>-143</v>
+      </c>
+      <c r="D15" s="2">
+        <v>-150.5</v>
+      </c>
+      <c r="E15" s="3">
+        <v>32</v>
+      </c>
+      <c r="F15" s="2">
+        <v>-92.5</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>